<commit_message>
Update flight computer v2 bom.xlsx
</commit_message>
<xml_diff>
--- a/flight_computer/v2/Bill of Material/flight computer v2 bom.xlsx
+++ b/flight_computer/v2/Bill of Material/flight computer v2 bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\internal-cubesat-boards\flight_computer\v2\Bill of Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63693185-2DA4-4FC8-8EBA-DF99249BB790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D6D340-3362-4827-B29A-64DB5DA66CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,9 +158,6 @@
     <t>Connector_Molex:Molex_PicoBlade_53047-1110_1x11_P1.25mm_Vertical</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/molex/0530471110/242862</t>
-  </si>
-  <si>
     <t xml:space="preserve">J11, </t>
   </si>
   <si>
@@ -473,9 +470,6 @@
     <t>Perovskite connector</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/molex/0510211100/242851</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/SR732BTTDR51J/12749611?s=N4IgTCBcDaIMoCUDsBmMAhAKpgIggrAIwBSIAugL5A</t>
   </si>
   <si>
@@ -540,6 +534,12 @@
   </si>
   <si>
     <t>External Debug</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/hirose-electric-co-ltd/DF13-11P-1-25DSA-05/15997313</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/hirose-electric-co-ltd/DF13-11S-1-25C/241760?s=N4IgjCBcoBw1oDGUBmBDANgZwKYBoQB7KAbRAHYAWGAJgDYQBdAgBwBcoQBlNgJwEsAdgHMQAXzEEapEABMUYAMxMxQA</t>
   </si>
 </sst>
 </file>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -904,7 +904,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -924,10 +924,10 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -944,7 +944,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
@@ -964,7 +964,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>12</v>
@@ -984,7 +984,7 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
@@ -1004,7 +1004,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>19</v>
@@ -1024,7 +1024,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>22</v>
@@ -1044,7 +1044,7 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>26</v>
@@ -1052,47 +1052,47 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
         <v>69</v>
       </c>
-      <c r="D9" t="s">
-        <v>70</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="4">
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" t="s">
-        <v>164</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="4">
         <v>17</v>
@@ -1101,58 +1101,58 @@
         <v>470</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="4">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
         <v>76</v>
       </c>
-      <c r="D12" t="s">
-        <v>77</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="4">
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B14" s="4">
         <v>4</v>
@@ -1161,18 +1161,18 @@
         <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" s="4">
         <v>4</v>
@@ -1181,18 +1181,18 @@
         <v>270</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" s="4">
         <v>4</v>
@@ -1201,73 +1201,73 @@
         <v>430</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B17" s="4">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>135</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>159</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="E19" t="s">
-        <v>161</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1278,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D20" t="s">
         <v>34</v>
@@ -1295,7 +1295,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
@@ -1312,7 +1312,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D22" t="s">
         <v>38</v>
@@ -1323,13 +1323,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>44</v>
-      </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>45</v>
       </c>
       <c r="D23" t="s">
         <v>34</v>
@@ -1340,13 +1340,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
         <v>46</v>
-      </c>
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>47</v>
       </c>
       <c r="D24" t="s">
         <v>34</v>
@@ -1357,291 +1357,291 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="4">
         <v>5</v>
       </c>
       <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
         <v>53</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="4">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>57</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>61</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="4">
         <v>3</v>
       </c>
       <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" t="s">
         <v>65</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="4">
         <v>2</v>
       </c>
       <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
         <v>86</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="4">
         <v>2</v>
       </c>
       <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
         <v>90</v>
       </c>
-      <c r="D30" t="s">
+      <c r="F30" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>163</v>
+      </c>
+      <c r="D31" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="F31" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>97</v>
       </c>
-      <c r="D32" t="s">
+      <c r="F32" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
         <v>100</v>
       </c>
-      <c r="B33" s="4">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>101</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F33" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>105</v>
       </c>
-      <c r="D34" t="s">
+      <c r="F34" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B35" s="4">
         <v>5</v>
       </c>
       <c r="C35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" t="s">
         <v>109</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F35" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B36" s="4">
         <v>16</v>
       </c>
       <c r="C36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" t="s">
         <v>113</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F36" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B37" s="4">
         <v>4</v>
       </c>
       <c r="C37" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D37" t="s">
-        <v>106</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="4">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>120</v>
       </c>
-      <c r="D38" t="s">
+      <c r="F38" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
         <v>123</v>
       </c>
-      <c r="B39" s="4">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
+        <v>90</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D39" t="s">
-        <v>91</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B40" s="4">
         <v>2</v>
       </c>
       <c r="C40" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" t="s">
         <v>127</v>
       </c>
-      <c r="D40" t="s">
+      <c r="F40" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B41" s="4">
         <v>18</v>
       </c>
       <c r="C41" t="s">
+        <v>130</v>
+      </c>
+      <c r="D41" t="s">
         <v>131</v>
       </c>
-      <c r="D41" t="s">
+      <c r="F41" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +1696,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1710,7 +1710,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1736,41 +1736,41 @@
         <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
       </c>
       <c r="D3" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>43</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>50</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>43</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1781,7 +1781,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
         <v>31</v>
@@ -1798,7 +1798,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
@@ -1809,11 +1809,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{361B5AA2-6605-4783-A432-CCBD220617F0}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{0B218452-1FF3-495A-AAD1-5C070A3C6293}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{3C426812-CA5E-4E11-9660-D630CD25173A}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{18C9A98E-047C-40C4-80AE-F49142AC854C}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{B49F7D83-CA68-496A-9258-1A8C4630018C}"/>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{18C9A98E-047C-40C4-80AE-F49142AC854C}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{B49F7D83-CA68-496A-9258-1A8C4630018C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1824,7 +1821,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1835,21 +1832,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" t="s">
         <v>141</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
         <v>142</v>
-      </c>
-      <c r="C1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1858,12 +1855,12 @@
         <v>100</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1872,12 +1869,12 @@
         <v>100</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1886,14 +1883,13 @@
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{BFC050C6-8070-4BD2-8F54-1AACD40F181A}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{A090880E-0DD6-49F9-B4A4-6055324608D2}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{4F249616-1CDD-4D68-B988-12E28D697A7F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create v3 flight computer
</commit_message>
<xml_diff>
--- a/flight_computer/v2/Bill of Material/flight computer v2 bom.xlsx
+++ b/flight_computer/v2/Bill of Material/flight computer v2 bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\internal-cubesat-boards\flight_computer\v2\Bill of Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D6D340-3362-4827-B29A-64DB5DA66CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43E5684-DD1F-4C6B-88C7-94B0E088EB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>